<commit_message>
criando coluna de servidor pra saber quem é servidor e quem é funcionario
</commit_message>
<xml_diff>
--- a/Tabela ponto servidores.xlsx
+++ b/Tabela ponto servidores.xlsx
@@ -279,22 +279,22 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>417240</xdr:colOff>
+      <xdr:colOff>208080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>681120</xdr:rowOff>
+      <xdr:rowOff>757080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -303,8 +303,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10440" y="0"/>
-          <a:ext cx="1867320" cy="681120"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1668600" cy="757080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8:G38"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>